<commit_message>
Updated pivot table with bank code
</commit_message>
<xml_diff>
--- a/section2/ChrisF_ExcelHomework.xlsx
+++ b/section2/ChrisF_ExcelHomework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Code\SavvyCoders\Homework\section2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6253496-8778-4D28-8BA9-D0F4C2C1B089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6F971F-7A35-4022-8A7D-639DEDB45BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29325" yWindow="1665" windowWidth="26970" windowHeight="13845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="456" windowWidth="21324" windowHeight="11712" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="173">
   <si>
     <t>Expenses</t>
   </si>
@@ -677,7 +677,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -740,6 +740,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -747,7 +750,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="17">
     <dxf>
       <alignment wrapText="1"/>
     </dxf>
@@ -755,82 +758,10 @@
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
     </dxf>
     <dxf>
       <font>
@@ -1750,6 +1681,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-008D-453F-9958-B72953EC7233}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1769,6 +1705,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-008D-453F-9958-B72953EC7233}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1788,6 +1729,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-008D-453F-9958-B72953EC7233}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1807,6 +1753,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-008D-453F-9958-B72953EC7233}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1826,6 +1777,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-008D-453F-9958-B72953EC7233}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2074,7 +2030,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[ExcelHomework.xlsx]Payments!PivotTable6</c:name>
+    <c:name>[ChrisF_ExcelHomework.xlsx]Payments!PivotTable6</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -2240,14 +2196,34 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Payments!$A$4:$A$8</c:f>
+              <c:f>Payments!$A$4:$A$14</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>B1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>B2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>B1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>B2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Jan</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="3">
                     <c:v>Feb</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2266,15 +2242,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Payments!$B$4:$B$8</c:f>
+              <c:f>Payments!$B$4:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>30301.25</c:v>
+                  <c:v>30270.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34664</c:v>
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34624</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4365,16 +4353,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>88582</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>11429</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>27622</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>382905</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>169545</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4427,7 +4415,11 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Bank Code" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="3">
+        <s v="B1"/>
+        <s v="B2"/>
+        <s v="PC"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Account Code" numFmtId="0">
       <sharedItems/>
@@ -4607,7 +4599,7 @@
     <s v="Opening Balance"/>
     <n v="5100"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-500"/>
     <x v="0"/>
   </r>
@@ -4618,7 +4610,7 @@
     <s v="Internet Service Provider"/>
     <n v="179"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-380"/>
     <x v="1"/>
   </r>
@@ -4629,7 +4621,7 @@
     <s v="Subscriptions"/>
     <n v="478"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-375"/>
     <x v="2"/>
   </r>
@@ -4640,7 +4632,7 @@
     <s v="Insurance"/>
     <n v="340"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-340"/>
     <x v="3"/>
   </r>
@@ -4651,7 +4643,7 @@
     <s v="Service Fees"/>
     <n v="50"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-315"/>
     <x v="4"/>
   </r>
@@ -4662,7 +4654,7 @@
     <s v="Service Fees"/>
     <n v="35"/>
     <s v="A"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-315"/>
     <x v="4"/>
   </r>
@@ -4673,7 +4665,7 @@
     <s v="Bookkeeping"/>
     <n v="1000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-305"/>
     <x v="5"/>
   </r>
@@ -4684,7 +4676,7 @@
     <s v="Flowers"/>
     <n v="90"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-345"/>
     <x v="4"/>
   </r>
@@ -4695,7 +4687,7 @@
     <s v="Parking"/>
     <n v="200"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-390"/>
     <x v="6"/>
   </r>
@@ -4706,7 +4698,7 @@
     <s v="Inter Account Transfer"/>
     <n v="-15000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="BS-399"/>
     <x v="7"/>
   </r>
@@ -4717,7 +4709,7 @@
     <s v="Inter Account Transfer"/>
     <n v="15000"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="7"/>
   </r>
@@ -4728,7 +4720,7 @@
     <s v="Salaries"/>
     <n v="13000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-365"/>
     <x v="8"/>
   </r>
@@ -4739,7 +4731,7 @@
     <s v="Capital repayment"/>
     <n v="220"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-700"/>
     <x v="8"/>
   </r>
@@ -4750,7 +4742,7 @@
     <s v="Interest paid"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-500"/>
     <x v="8"/>
   </r>
@@ -4761,7 +4753,7 @@
     <s v="Rent"/>
     <n v="6400"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-350"/>
     <x v="8"/>
   </r>
@@ -4772,7 +4764,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="1"/>
   </r>
@@ -4783,7 +4775,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="-100"/>
     <s v="E"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="BS-399"/>
     <x v="1"/>
   </r>
@@ -4794,7 +4786,7 @@
     <s v="Internet Service Provider"/>
     <n v="179"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-380"/>
     <x v="9"/>
   </r>
@@ -4805,7 +4797,7 @@
     <s v="Insurance"/>
     <n v="340"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-340"/>
     <x v="10"/>
   </r>
@@ -4816,7 +4808,7 @@
     <s v="Flowers"/>
     <n v="87"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-345"/>
     <x v="11"/>
   </r>
@@ -4827,7 +4819,7 @@
     <s v="Service Fees"/>
     <n v="80"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-315"/>
     <x v="12"/>
   </r>
@@ -4838,7 +4830,7 @@
     <s v="Service Fees"/>
     <n v="35"/>
     <s v="A"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-315"/>
     <x v="12"/>
   </r>
@@ -4849,7 +4841,7 @@
     <s v="Bookkeeping"/>
     <n v="1000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-305"/>
     <x v="13"/>
   </r>
@@ -4860,7 +4852,7 @@
     <s v="Inter Account Transfer"/>
     <n v="-20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="BS-399"/>
     <x v="14"/>
   </r>
@@ -4871,7 +4863,7 @@
     <s v="Inter Account Transfer"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="14"/>
   </r>
@@ -4882,7 +4874,7 @@
     <s v="Sales Tax"/>
     <n v="1300"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-600"/>
     <x v="15"/>
   </r>
@@ -4893,7 +4885,7 @@
     <s v="Salaries"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-365"/>
     <x v="16"/>
   </r>
@@ -4904,7 +4896,7 @@
     <s v="Furniture"/>
     <n v="3000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-100"/>
     <x v="17"/>
   </r>
@@ -4915,7 +4907,7 @@
     <s v="Capital repayment"/>
     <n v="220"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-700"/>
     <x v="16"/>
   </r>
@@ -4926,7 +4918,7 @@
     <s v="Interest paid"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-500"/>
     <x v="16"/>
   </r>
@@ -4937,7 +4929,7 @@
     <s v="Rent"/>
     <n v="6400"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-350"/>
     <x v="16"/>
   </r>
@@ -4948,7 +4940,7 @@
     <s v="Consumables"/>
     <n v="41"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-325"/>
     <x v="18"/>
   </r>
@@ -4959,7 +4951,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="19"/>
   </r>
@@ -4970,7 +4962,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="-100"/>
     <s v="E"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="BS-399"/>
     <x v="19"/>
   </r>
@@ -4981,7 +4973,7 @@
     <s v="Internet Service Provider"/>
     <n v="179"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-380"/>
     <x v="20"/>
   </r>
@@ -4992,7 +4984,7 @@
     <s v="Course"/>
     <n v="220"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-385"/>
     <x v="20"/>
   </r>
@@ -5003,7 +4995,7 @@
     <s v="Insurance"/>
     <n v="340"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-340"/>
     <x v="21"/>
   </r>
@@ -5014,7 +5006,7 @@
     <s v="Accommodation"/>
     <n v="563"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-390"/>
     <x v="22"/>
   </r>
@@ -5025,7 +5017,7 @@
     <s v="Stationery"/>
     <n v="982"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-370"/>
     <x v="23"/>
   </r>
@@ -5036,7 +5028,7 @@
     <s v="Service Fees"/>
     <n v="80"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-315"/>
     <x v="24"/>
   </r>
@@ -5047,7 +5039,7 @@
     <s v="Service Fees"/>
     <n v="35"/>
     <s v="A"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-315"/>
     <x v="24"/>
   </r>
@@ -5058,7 +5050,7 @@
     <s v="Bookkeeping"/>
     <n v="1000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-305"/>
     <x v="25"/>
   </r>
@@ -5069,7 +5061,7 @@
     <s v="Inter Account Transfer"/>
     <n v="-20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="BS-399"/>
     <x v="26"/>
   </r>
@@ -5080,7 +5072,7 @@
     <s v="Inter Account Transfer"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="26"/>
   </r>
@@ -5091,7 +5083,7 @@
     <s v="Salaries"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-365"/>
     <x v="17"/>
   </r>
@@ -5102,7 +5094,7 @@
     <s v="Capital repayment"/>
     <n v="220"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-700"/>
     <x v="17"/>
   </r>
@@ -5113,7 +5105,7 @@
     <s v="Interest paid"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-500"/>
     <x v="17"/>
   </r>
@@ -5124,7 +5116,7 @@
     <s v="Rent"/>
     <n v="6400"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-350"/>
     <x v="17"/>
   </r>
@@ -5135,7 +5127,7 @@
     <s v="Flowers"/>
     <n v="65"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-345"/>
     <x v="18"/>
   </r>
@@ -5146,7 +5138,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="20"/>
   </r>
@@ -5157,7 +5149,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="-100"/>
     <s v="E"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="BS-399"/>
     <x v="20"/>
   </r>
@@ -5168,7 +5160,7 @@
     <s v="Internet Service Provider"/>
     <n v="179"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-380"/>
     <x v="27"/>
   </r>
@@ -5179,7 +5171,7 @@
     <s v="Insurance"/>
     <n v="340"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-340"/>
     <x v="28"/>
   </r>
@@ -5190,7 +5182,7 @@
     <s v="Service Fees"/>
     <n v="80"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-315"/>
     <x v="29"/>
   </r>
@@ -5201,7 +5193,7 @@
     <s v="Service Fees"/>
     <n v="35"/>
     <s v="A"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-315"/>
     <x v="29"/>
   </r>
@@ -5212,7 +5204,7 @@
     <s v="Bookkeeping"/>
     <n v="1000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-305"/>
     <x v="30"/>
   </r>
@@ -5223,7 +5215,7 @@
     <s v="Inter Account Transfer"/>
     <n v="-20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="BS-399"/>
     <x v="31"/>
   </r>
@@ -5234,7 +5226,7 @@
     <s v="Inter Account Transfer"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="31"/>
   </r>
@@ -5245,7 +5237,7 @@
     <s v="Flowers"/>
     <n v="110"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-345"/>
     <x v="32"/>
   </r>
@@ -5256,7 +5248,7 @@
     <s v="Sales Tax"/>
     <n v="8700"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-600"/>
     <x v="33"/>
   </r>
@@ -5267,7 +5259,7 @@
     <s v="Salaries"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-365"/>
     <x v="34"/>
   </r>
@@ -5278,7 +5270,7 @@
     <s v="Capital repayment"/>
     <n v="220"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-700"/>
     <x v="34"/>
   </r>
@@ -5289,7 +5281,7 @@
     <s v="Interest paid"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-500"/>
     <x v="34"/>
   </r>
@@ -5300,7 +5292,7 @@
     <s v="Rent"/>
     <n v="6400"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-350"/>
     <x v="34"/>
   </r>
@@ -5311,7 +5303,7 @@
     <s v="Travel"/>
     <n v="1782"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-390"/>
     <x v="34"/>
   </r>
@@ -5322,7 +5314,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="35"/>
   </r>
@@ -5333,7 +5325,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="-100"/>
     <s v="E"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="BS-399"/>
     <x v="35"/>
   </r>
@@ -5344,7 +5336,7 @@
     <s v="Internet Service Provider"/>
     <n v="179"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-380"/>
     <x v="36"/>
   </r>
@@ -5355,7 +5347,7 @@
     <s v="Stationery"/>
     <n v="761"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-370"/>
     <x v="37"/>
   </r>
@@ -5366,7 +5358,7 @@
     <s v="Insurance"/>
     <n v="340"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-340"/>
     <x v="38"/>
   </r>
@@ -5377,7 +5369,7 @@
     <s v="Service Fees"/>
     <n v="80"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-315"/>
     <x v="39"/>
   </r>
@@ -5388,7 +5380,7 @@
     <s v="Service Fees"/>
     <n v="35"/>
     <s v="A"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-315"/>
     <x v="39"/>
   </r>
@@ -5399,7 +5391,7 @@
     <s v="Bookkeeping"/>
     <n v="1000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-305"/>
     <x v="40"/>
   </r>
@@ -5410,7 +5402,7 @@
     <s v="Flowers"/>
     <n v="29"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-345"/>
     <x v="41"/>
   </r>
@@ -5421,7 +5413,7 @@
     <s v="Consumables"/>
     <n v="937"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-325"/>
     <x v="42"/>
   </r>
@@ -5432,7 +5424,7 @@
     <s v="Inter Account Transfer"/>
     <n v="-20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="BS-399"/>
     <x v="43"/>
   </r>
@@ -5443,7 +5435,7 @@
     <s v="Inter Account Transfer"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="43"/>
   </r>
@@ -5454,7 +5446,7 @@
     <s v="Annual Membership"/>
     <n v="2000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-375"/>
     <x v="44"/>
   </r>
@@ -5465,7 +5457,7 @@
     <s v="Salaries"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-365"/>
     <x v="45"/>
   </r>
@@ -5476,7 +5468,7 @@
     <s v="Capital repayment"/>
     <n v="220"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-700"/>
     <x v="45"/>
   </r>
@@ -5487,7 +5479,7 @@
     <s v="Interest paid"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-500"/>
     <x v="45"/>
   </r>
@@ -5498,7 +5490,7 @@
     <s v="Rent"/>
     <n v="6400"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-350"/>
     <x v="45"/>
   </r>
@@ -5509,7 +5501,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="50"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="36"/>
   </r>
@@ -5520,7 +5512,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="-50"/>
     <s v="E"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="BS-399"/>
     <x v="36"/>
   </r>
@@ -5531,7 +5523,7 @@
     <s v="Internet Service Provider"/>
     <n v="179"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-380"/>
     <x v="46"/>
   </r>
@@ -5542,7 +5534,7 @@
     <s v="Insurance"/>
     <n v="340"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-340"/>
     <x v="47"/>
   </r>
@@ -5553,7 +5545,7 @@
     <s v="Flowers"/>
     <n v="78"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-345"/>
     <x v="48"/>
   </r>
@@ -5564,7 +5556,7 @@
     <s v="Commission"/>
     <n v="747"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-320"/>
     <x v="49"/>
   </r>
@@ -5575,7 +5567,7 @@
     <s v="Service Fees"/>
     <n v="80"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-315"/>
     <x v="50"/>
   </r>
@@ -5586,7 +5578,7 @@
     <s v="Service Fees"/>
     <n v="35"/>
     <s v="A"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-315"/>
     <x v="50"/>
   </r>
@@ -5597,7 +5589,7 @@
     <s v="Bookkeeping"/>
     <n v="1000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-305"/>
     <x v="51"/>
   </r>
@@ -5608,7 +5600,7 @@
     <s v="Travel"/>
     <n v="1278"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-390"/>
     <x v="50"/>
   </r>
@@ -5619,7 +5611,7 @@
     <s v="Inter Account Transfer"/>
     <n v="-20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="BS-399"/>
     <x v="52"/>
   </r>
@@ -5630,7 +5622,7 @@
     <s v="Inter Account Transfer"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="52"/>
   </r>
@@ -5641,7 +5633,7 @@
     <s v="Share investment"/>
     <n v="3750"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-200"/>
     <x v="53"/>
   </r>
@@ -5652,7 +5644,7 @@
     <s v="Sales Tax"/>
     <n v="6600"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-600"/>
     <x v="54"/>
   </r>
@@ -5663,7 +5655,7 @@
     <s v="Salaries"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-365"/>
     <x v="55"/>
   </r>
@@ -5674,7 +5666,7 @@
     <s v="Capital repayment"/>
     <n v="220"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-700"/>
     <x v="55"/>
   </r>
@@ -5685,7 +5677,7 @@
     <s v="Interest paid"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-500"/>
     <x v="55"/>
   </r>
@@ -5696,7 +5688,7 @@
     <s v="Rent"/>
     <n v="6400"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-350"/>
     <x v="55"/>
   </r>
@@ -5707,7 +5699,7 @@
     <s v="Stationery"/>
     <n v="234"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-370"/>
     <x v="56"/>
   </r>
@@ -5718,7 +5710,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="50"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="46"/>
   </r>
@@ -5729,7 +5721,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="-50"/>
     <s v="E"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="BS-399"/>
     <x v="46"/>
   </r>
@@ -5740,7 +5732,7 @@
     <s v="Provisional Tax"/>
     <n v="2600"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-600"/>
     <x v="46"/>
   </r>
@@ -5751,7 +5743,7 @@
     <s v="Internet Service Provider"/>
     <n v="179"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-380"/>
     <x v="57"/>
   </r>
@@ -5762,7 +5754,7 @@
     <s v="Insurance"/>
     <n v="340"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-340"/>
     <x v="58"/>
   </r>
@@ -5773,7 +5765,7 @@
     <s v="Course"/>
     <n v="277.48"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-385"/>
     <x v="59"/>
   </r>
@@ -5784,7 +5776,7 @@
     <s v="Service Fees"/>
     <n v="80"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-315"/>
     <x v="60"/>
   </r>
@@ -5795,7 +5787,7 @@
     <s v="Service Fees"/>
     <n v="35"/>
     <s v="A"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-315"/>
     <x v="60"/>
   </r>
@@ -5806,7 +5798,7 @@
     <s v="Bookkeeping"/>
     <n v="1000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-305"/>
     <x v="61"/>
   </r>
@@ -5817,7 +5809,7 @@
     <s v="Rates"/>
     <n v="5620"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-395"/>
     <x v="62"/>
   </r>
@@ -5828,7 +5820,7 @@
     <s v="Legal advice"/>
     <n v="12500"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-360"/>
     <x v="62"/>
   </r>
@@ -5839,7 +5831,7 @@
     <s v="Inter Account Transfer"/>
     <n v="-20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="BS-399"/>
     <x v="63"/>
   </r>
@@ -5850,7 +5842,7 @@
     <s v="Inter Account Transfer"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="63"/>
   </r>
@@ -5861,7 +5853,7 @@
     <s v="Flowers"/>
     <n v="90"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-345"/>
     <x v="64"/>
   </r>
@@ -5872,7 +5864,7 @@
     <s v="Commission"/>
     <n v="4242"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-320"/>
     <x v="65"/>
   </r>
@@ -5883,7 +5875,7 @@
     <s v="Salaries"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-365"/>
     <x v="56"/>
   </r>
@@ -5894,7 +5886,7 @@
     <s v="Capital repayment"/>
     <n v="220"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-700"/>
     <x v="56"/>
   </r>
@@ -5905,7 +5897,7 @@
     <s v="Interest paid"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-500"/>
     <x v="56"/>
   </r>
@@ -5916,7 +5908,7 @@
     <s v="Rent"/>
     <n v="6400"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-350"/>
     <x v="56"/>
   </r>
@@ -5927,7 +5919,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="66"/>
   </r>
@@ -5938,7 +5930,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="-100"/>
     <s v="E"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="BS-399"/>
     <x v="66"/>
   </r>
@@ -5949,7 +5941,7 @@
     <s v="Internet Service Provider"/>
     <n v="179"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-380"/>
     <x v="67"/>
   </r>
@@ -5960,7 +5952,7 @@
     <s v="Consumables"/>
     <n v="62"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-325"/>
     <x v="68"/>
   </r>
@@ -5971,7 +5963,7 @@
     <s v="Travel"/>
     <n v="1887"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-390"/>
     <x v="69"/>
   </r>
@@ -5982,7 +5974,7 @@
     <s v="Insurance"/>
     <n v="340"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-340"/>
     <x v="70"/>
   </r>
@@ -5993,7 +5985,7 @@
     <s v="Service Fees"/>
     <n v="80"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-315"/>
     <x v="71"/>
   </r>
@@ -6004,7 +5996,7 @@
     <s v="Service Fees"/>
     <n v="35"/>
     <s v="A"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-315"/>
     <x v="71"/>
   </r>
@@ -6015,7 +6007,7 @@
     <s v="Bookkeeping"/>
     <n v="1000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-305"/>
     <x v="72"/>
   </r>
@@ -6026,7 +6018,7 @@
     <s v="Inter Account Transfer"/>
     <n v="-20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="BS-399"/>
     <x v="73"/>
   </r>
@@ -6037,7 +6029,7 @@
     <s v="Inter Account Transfer"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="73"/>
   </r>
@@ -6048,7 +6040,7 @@
     <s v="Stationery"/>
     <n v="289"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-370"/>
     <x v="74"/>
   </r>
@@ -6059,7 +6051,7 @@
     <s v="Sales Tax"/>
     <n v="3300"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-600"/>
     <x v="75"/>
   </r>
@@ -6070,7 +6062,7 @@
     <s v="Salaries"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-365"/>
     <x v="76"/>
   </r>
@@ -6081,7 +6073,7 @@
     <s v="Capital repayment"/>
     <n v="220"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-700"/>
     <x v="76"/>
   </r>
@@ -6092,7 +6084,7 @@
     <s v="Interest paid"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-500"/>
     <x v="76"/>
   </r>
@@ -6103,7 +6095,7 @@
     <s v="Rent"/>
     <n v="6400"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-350"/>
     <x v="76"/>
   </r>
@@ -6114,7 +6106,7 @@
     <s v="Flowers"/>
     <n v="218"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-345"/>
     <x v="77"/>
   </r>
@@ -6125,7 +6117,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="200"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="67"/>
   </r>
@@ -6136,7 +6128,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="-200"/>
     <s v="E"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="BS-399"/>
     <x v="67"/>
   </r>
@@ -6147,7 +6139,7 @@
     <s v="Internet Service Provider"/>
     <n v="179"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-380"/>
     <x v="78"/>
   </r>
@@ -6158,7 +6150,7 @@
     <s v="Insurance"/>
     <n v="340"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-340"/>
     <x v="79"/>
   </r>
@@ -6169,7 +6161,7 @@
     <s v="Commission"/>
     <n v="982"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-320"/>
     <x v="80"/>
   </r>
@@ -6180,7 +6172,7 @@
     <s v="Service Fees"/>
     <n v="80"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-315"/>
     <x v="81"/>
   </r>
@@ -6191,7 +6183,7 @@
     <s v="Service Fees"/>
     <n v="35"/>
     <s v="A"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-315"/>
     <x v="81"/>
   </r>
@@ -6202,7 +6194,7 @@
     <s v="Bookkeeping"/>
     <n v="1000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-305"/>
     <x v="82"/>
   </r>
@@ -6213,7 +6205,7 @@
     <s v="Flowers"/>
     <n v="102"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-345"/>
     <x v="83"/>
   </r>
@@ -6224,7 +6216,7 @@
     <s v="Inter Account Transfer"/>
     <n v="-20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="BS-399"/>
     <x v="84"/>
   </r>
@@ -6235,7 +6227,7 @@
     <s v="Inter Account Transfer"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="84"/>
   </r>
@@ -6246,7 +6238,7 @@
     <s v="Salaries"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-365"/>
     <x v="85"/>
   </r>
@@ -6257,7 +6249,7 @@
     <s v="Capital repayment"/>
     <n v="220"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-700"/>
     <x v="85"/>
   </r>
@@ -6268,7 +6260,7 @@
     <s v="Interest paid"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-500"/>
     <x v="85"/>
   </r>
@@ -6279,7 +6271,7 @@
     <s v="Rent"/>
     <n v="6400"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-350"/>
     <x v="85"/>
   </r>
@@ -6290,7 +6282,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="170"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="86"/>
   </r>
@@ -6301,7 +6293,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="-170"/>
     <s v="E"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="BS-399"/>
     <x v="86"/>
   </r>
@@ -6312,7 +6304,7 @@
     <s v="Internet Service Provider"/>
     <n v="179"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-380"/>
     <x v="87"/>
   </r>
@@ -6323,7 +6315,7 @@
     <s v="Insurance"/>
     <n v="340"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-340"/>
     <x v="80"/>
   </r>
@@ -6334,7 +6326,7 @@
     <s v="Flowers"/>
     <n v="96"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-345"/>
     <x v="88"/>
   </r>
@@ -6345,7 +6337,7 @@
     <s v="Service Fees"/>
     <n v="80"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-315"/>
     <x v="89"/>
   </r>
@@ -6356,7 +6348,7 @@
     <s v="Service Fees"/>
     <n v="35"/>
     <s v="A"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-315"/>
     <x v="89"/>
   </r>
@@ -6367,7 +6359,7 @@
     <s v="Bookkeeping"/>
     <n v="1000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-305"/>
     <x v="90"/>
   </r>
@@ -6378,7 +6370,7 @@
     <s v="Subscriptions"/>
     <n v="120"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-375"/>
     <x v="91"/>
   </r>
@@ -6389,7 +6381,7 @@
     <s v="Stationery"/>
     <n v="310"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-370"/>
     <x v="91"/>
   </r>
@@ -6400,7 +6392,7 @@
     <s v="Commission"/>
     <n v="962"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-320"/>
     <x v="91"/>
   </r>
@@ -6411,7 +6403,7 @@
     <s v="Inter Account Transfer"/>
     <n v="-20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="BS-399"/>
     <x v="92"/>
   </r>
@@ -6422,7 +6414,7 @@
     <s v="Inter Account Transfer"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="92"/>
   </r>
@@ -6433,7 +6425,7 @@
     <s v="Consumables"/>
     <n v="61"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-325"/>
     <x v="93"/>
   </r>
@@ -6444,7 +6436,7 @@
     <s v="Sales Tax"/>
     <n v="8400"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-600"/>
     <x v="94"/>
   </r>
@@ -6455,7 +6447,7 @@
     <s v="Salaries"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-365"/>
     <x v="95"/>
   </r>
@@ -6466,7 +6458,7 @@
     <s v="Capital repayment"/>
     <n v="220"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-700"/>
     <x v="95"/>
   </r>
@@ -6477,7 +6469,7 @@
     <s v="Interest paid"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-500"/>
     <x v="95"/>
   </r>
@@ -6488,7 +6480,7 @@
     <s v="Rent"/>
     <n v="6400"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-350"/>
     <x v="95"/>
   </r>
@@ -6499,7 +6491,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="87"/>
   </r>
@@ -6510,7 +6502,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="-100"/>
     <s v="E"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="BS-399"/>
     <x v="87"/>
   </r>
@@ -6521,7 +6513,7 @@
     <s v="Internet Service Provider"/>
     <n v="179"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-380"/>
     <x v="96"/>
   </r>
@@ -6532,7 +6524,7 @@
     <s v="Insurance"/>
     <n v="340"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-340"/>
     <x v="97"/>
   </r>
@@ -6543,7 +6535,7 @@
     <s v="Service Fees"/>
     <n v="80"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-315"/>
     <x v="98"/>
   </r>
@@ -6554,7 +6546,7 @@
     <s v="Service Fees"/>
     <n v="35"/>
     <s v="A"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-315"/>
     <x v="98"/>
   </r>
@@ -6565,7 +6557,7 @@
     <s v="Bookkeeping"/>
     <n v="1000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-305"/>
     <x v="99"/>
   </r>
@@ -6576,7 +6568,7 @@
     <s v="Flowers"/>
     <n v="105"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-345"/>
     <x v="91"/>
   </r>
@@ -6587,7 +6579,7 @@
     <s v="Inter Account Transfer"/>
     <n v="-20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="BS-399"/>
     <x v="100"/>
   </r>
@@ -6598,7 +6590,7 @@
     <s v="Inter Account Transfer"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="100"/>
   </r>
@@ -6609,7 +6601,7 @@
     <s v="Salaries"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-365"/>
     <x v="101"/>
   </r>
@@ -6620,7 +6612,7 @@
     <s v="Capital repayment"/>
     <n v="220"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-700"/>
     <x v="101"/>
   </r>
@@ -6631,7 +6623,7 @@
     <s v="Interest paid"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-500"/>
     <x v="101"/>
   </r>
@@ -6642,7 +6634,7 @@
     <s v="Rent"/>
     <n v="6400"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-350"/>
     <x v="101"/>
   </r>
@@ -6653,7 +6645,7 @@
     <s v="Training"/>
     <n v="389.25"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-385"/>
     <x v="96"/>
   </r>
@@ -6664,7 +6656,7 @@
     <s v="Commission"/>
     <n v="514"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-320"/>
     <x v="102"/>
   </r>
@@ -6675,7 +6667,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="170"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="96"/>
   </r>
@@ -6686,7 +6678,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="-170"/>
     <s v="E"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="BS-399"/>
     <x v="96"/>
   </r>
@@ -6697,7 +6689,7 @@
     <s v="Internet Service Provider"/>
     <n v="179"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-380"/>
     <x v="103"/>
   </r>
@@ -6708,7 +6700,7 @@
     <s v="Insurance"/>
     <n v="340"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-340"/>
     <x v="104"/>
   </r>
@@ -6719,7 +6711,7 @@
     <s v="Stationery"/>
     <n v="289"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-370"/>
     <x v="103"/>
   </r>
@@ -6730,7 +6722,7 @@
     <s v="Service Fees"/>
     <n v="80"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-315"/>
     <x v="105"/>
   </r>
@@ -6741,7 +6733,7 @@
     <s v="Service Fees"/>
     <n v="35"/>
     <s v="A"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-315"/>
     <x v="105"/>
   </r>
@@ -6752,7 +6744,7 @@
     <s v="Bookkeeping"/>
     <n v="1000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-305"/>
     <x v="103"/>
   </r>
@@ -6763,7 +6755,7 @@
     <s v="Inter Account Transfer"/>
     <n v="-20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="BS-399"/>
     <x v="106"/>
   </r>
@@ -6774,7 +6766,7 @@
     <s v="Inter Account Transfer"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="106"/>
   </r>
@@ -6785,7 +6777,7 @@
     <s v="Sales Tax"/>
     <n v="2200"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-600"/>
     <x v="107"/>
   </r>
@@ -6796,7 +6788,7 @@
     <s v="Flowers"/>
     <n v="75"/>
     <s v="A"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="IS-345"/>
     <x v="107"/>
   </r>
@@ -6807,7 +6799,7 @@
     <s v="Office equipment"/>
     <n v="10000"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-100"/>
     <x v="103"/>
   </r>
@@ -6818,7 +6810,7 @@
     <s v="Salaries"/>
     <n v="20000"/>
     <s v="E"/>
-    <s v="B2"/>
+    <x v="1"/>
     <s v="IS-365"/>
     <x v="108"/>
   </r>
@@ -6829,7 +6821,7 @@
     <s v="Capital repayment"/>
     <n v="220"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-700"/>
     <x v="108"/>
   </r>
@@ -6840,7 +6832,7 @@
     <s v="Interest paid"/>
     <n v="100"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-500"/>
     <x v="108"/>
   </r>
@@ -6851,7 +6843,7 @@
     <s v="Rent"/>
     <n v="6400"/>
     <s v="A"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-350"/>
     <x v="108"/>
   </r>
@@ -6862,7 +6854,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="70"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="BS-399"/>
     <x v="109"/>
   </r>
@@ -6873,7 +6865,7 @@
     <s v="Petty Cash Reimbursement"/>
     <n v="-70"/>
     <s v="E"/>
-    <s v="PC"/>
+    <x v="2"/>
     <s v="BS-399"/>
     <x v="109"/>
   </r>
@@ -6884,7 +6876,7 @@
     <s v="Provisional Tax"/>
     <n v="3700"/>
     <s v="E"/>
-    <s v="B1"/>
+    <x v="0"/>
     <s v="IS-600"/>
     <x v="109"/>
   </r>
@@ -6892,8 +6884,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5BD7C614-9F3D-4318-8A3D-E92C5709C969}" name="PivotTable6" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5BD7C614-9F3D-4318-8A3D-E92C5709C969}" name="PivotTable6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField showAll="0"/>
@@ -6901,7 +6893,14 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" numFmtId="43" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="15">
@@ -6943,12 +6942,13 @@
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="3">
+  <rowFields count="4">
     <field x="10"/>
     <field x="9"/>
     <field x="8"/>
+    <field x="6"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="11">
     <i>
       <x v="2"/>
     </i>
@@ -6958,7 +6958,25 @@
     <i r="2">
       <x v="1"/>
     </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x v="2"/>
+    </i>
     <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="3">
       <x v="2"/>
     </i>
     <i t="grand">
@@ -6972,10 +6990,10 @@
     <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="10" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="8">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -7016,18 +7034,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E8CA7A42-88D3-4BA9-8773-A48845F6A148}" name="Table3" displayName="Table3" ref="A2:I210" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E8CA7A42-88D3-4BA9-8773-A48845F6A148}" name="Table3" displayName="Table3" ref="A2:I210" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
   <autoFilter ref="A2:I210" xr:uid="{E8CA7A42-88D3-4BA9-8773-A48845F6A148}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{4D06A3E9-AC55-42F5-B97A-CF1BB891A0EF}" name="Document Date" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{19C072D9-AA0C-403D-8F96-DFDFAE3C9C13}" name="Supplier" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{528F7C03-E113-423C-9716-CD409FAFF084}" name="Reference" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{A585D1DD-700E-4823-A63A-B4DFD533DD91}" name="Description" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{3D811E8D-304B-4C4C-9790-38F431690F8E}" name="Tax Inclusive Amount" dataDxfId="32" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{68D16422-4579-461A-A7AA-8277FD25C9CD}" name="Column1" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{D98B29F9-F512-4B41-906C-E592D6883E05}" name="Bank Code" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{21BAFC6F-2881-4AC2-851A-41C8EA29568D}" name="Account Code" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{05162FE6-5D07-42E5-8701-2D3BD8C3C735}" name="Payment Date" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{4D06A3E9-AC55-42F5-B97A-CF1BB891A0EF}" name="Document Date" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{19C072D9-AA0C-403D-8F96-DFDFAE3C9C13}" name="Supplier" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{528F7C03-E113-423C-9716-CD409FAFF084}" name="Reference" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{A585D1DD-700E-4823-A63A-B4DFD533DD91}" name="Description" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{3D811E8D-304B-4C4C-9790-38F431690F8E}" name="Tax Inclusive Amount" dataDxfId="8" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{68D16422-4579-461A-A7AA-8277FD25C9CD}" name="Column1" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{D98B29F9-F512-4B41-906C-E592D6883E05}" name="Bank Code" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{21BAFC6F-2881-4AC2-851A-41C8EA29568D}" name="Account Code" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{05162FE6-5D07-42E5-8701-2D3BD8C3C735}" name="Payment Date" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7332,7 +7350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{469471DC-70BD-47B1-99A6-3FE5302BC7DC}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -7728,7 +7746,7 @@
         <v>1238.25</v>
       </c>
       <c r="G6" s="18">
-        <f t="shared" ref="G5:G8" si="2">F6/D6</f>
+        <f t="shared" ref="G6:G8" si="2">F6/D6</f>
         <v>412.75</v>
       </c>
     </row>
@@ -13882,10 +13900,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7698054C-9202-4D00-8BAF-E2CD8CC28B1A}">
-  <dimension ref="A3:B8"/>
+  <dimension ref="A3:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13926,18 +13944,66 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="27">
+        <v>30270.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="27">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="27">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B10" s="27">
         <v>34664</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="27">
+        <v>34624</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="27">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B14" s="27">
         <v>64965.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corrected issue with excel hw
</commit_message>
<xml_diff>
--- a/section2/ChrisF_ExcelHomework.xlsx
+++ b/section2/ChrisF_ExcelHomework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Code\SavvyCoders\Homework\section2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6F971F-7A35-4022-8A7D-639DEDB45BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06B761C-D333-47AD-B823-53DE7946482F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="456" windowWidth="21324" windowHeight="11712" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31350" yWindow="2550" windowWidth="21600" windowHeight="13185" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="174">
   <si>
     <t>Expenses</t>
   </si>
@@ -558,6 +558,9 @@
   </si>
   <si>
     <t>Citi Card</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
   </si>
 </sst>
 </file>
@@ -677,7 +680,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -736,13 +739,7 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2034,61 +2031,92 @@
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
         <c:spPr>
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:schemeClr val="accent1">
+              <a:alpha val="88000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
-          <a:sp3d/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="threePt" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:contourClr>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:contourClr>
+          </a:sp3d>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:spPr>
-            <a:noFill/>
+            <a:solidFill>
+              <a:srgbClr val="ED7D31">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:alpha val="50000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:txPr>
             <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
@@ -2097,12 +2125,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="lt1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2113,7 +2138,207 @@
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="88000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="threePt" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:contourClr>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="A5A5A5">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:alpha val="50000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="88000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="threePt" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:contourClr>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4472C4">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:alpha val="50000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2133,7 +2358,12 @@
     <c:floor>
       <c:thickness val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="75000"/>
+            <a:alpha val="27000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -2174,56 +2404,120 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Payments!$B$3</c:f>
+              <c:f>Payments!$B$3:$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Total</c:v>
+                  <c:v>B1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent1">
+                <a:alpha val="88000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d prstMaterial="flat">
+              <a:contourClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4472C4">
+                  <a:alpha val="30000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF">
+                    <a:alpha val="50000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Payments!$A$4:$A$14</c:f>
+              <c:f>Payments!$A$5:$A$9</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>B1</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>B2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>PC</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>B1</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>B2</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>PC</c:v>
-                  </c:pt>
-                </c:lvl>
+                <c:ptCount val="2"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Jan</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="1">
                     <c:v>Feb</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2242,27 +2536,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Payments!$B$4:$B$14</c:f>
+              <c:f>Payments!$B$5:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>30270.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>34624</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2273,15 +2555,328 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Payments!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>B2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:alpha val="88000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d prstMaterial="flat">
+              <a:contourClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ED7D31">
+                  <a:alpha val="30000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF">
+                    <a:alpha val="50000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Payments!$A$5:$A$9</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2012</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Payments!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AFD9-4B07-A4FD-940BEFA09790}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Payments!$D$3:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:alpha val="88000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:scene3d>
+              <a:camera prst="orthographicFront"/>
+              <a:lightRig rig="threePt" dir="t"/>
+            </a:scene3d>
+            <a:sp3d prstMaterial="flat">
+              <a:contourClr>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="A5A5A5">
+                  <a:alpha val="30000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF">
+                    <a:alpha val="50000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Payments!$A$5:$A$9</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2012</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Payments!$D$5:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AFD9-4B07-A4FD-940BEFA09790}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="84"/>
+        <c:gapDepth val="53"/>
         <c:shape val="box"/>
         <c:axId val="437839904"/>
         <c:axId val="386734816"/>
@@ -2312,9 +2907,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2337,53 +2931,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="437839904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -2413,9 +2966,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -2440,13 +2992,15 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
+        <a:schemeClr val="dk1">
+          <a:tint val="75000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -3779,47 +4333,47 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="291">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:chartArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:tint val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3829,69 +4383,135 @@
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="30000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="phClr">
+          <a:alpha val="30000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="88000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="88000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="flat"/>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -3906,10 +4526,8 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -3917,19 +4535,25 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -3948,21 +4572,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3972,20 +4593,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3997,14 +4617,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4016,14 +4635,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4038,10 +4656,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="bg2">
+          <a:lumMod val="75000"/>
+          <a:alpha val="27000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:sp3d/>
     </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
@@ -4052,14 +4673,12 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMajor>
@@ -4071,14 +4690,12 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -4087,14 +4704,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="lt1">
             <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4106,14 +4722,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4125,14 +4740,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -4140,7 +4754,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -4153,9 +4767,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4165,14 +4778,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4184,12 +4796,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1800" b="0" kern="1200" cap="all" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4198,14 +4807,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -4214,9 +4824,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4226,17 +4835,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4248,9 +4858,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4263,10 +4872,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
+      <a:sp3d/>
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
@@ -4353,16 +4959,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>27622</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>172403</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>382905</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>169545</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>53341</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6884,8 +7490,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5BD7C614-9F3D-4318-8A3D-E92C5709C969}" name="PivotTable6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5BD7C614-9F3D-4318-8A3D-E92C5709C969}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField showAll="0"/>
@@ -6893,7 +7499,7 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" numFmtId="43" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisCol" showAll="0">
       <items count="4">
         <item x="0"/>
         <item x="1"/>
@@ -6942,13 +7548,12 @@
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="4">
+  <rowFields count="3">
     <field x="10"/>
     <field x="9"/>
     <field x="8"/>
-    <field x="6"/>
   </rowFields>
-  <rowItems count="11">
+  <rowItems count="5">
     <i>
       <x v="2"/>
     </i>
@@ -6958,33 +7563,29 @@
     <i r="2">
       <x v="1"/>
     </i>
-    <i r="3">
-      <x/>
-    </i>
-    <i r="3">
-      <x v="1"/>
-    </i>
-    <i r="3">
-      <x v="2"/>
-    </i>
     <i r="2">
-      <x v="2"/>
-    </i>
-    <i r="3">
-      <x/>
-    </i>
-    <i r="3">
-      <x v="1"/>
-    </i>
-    <i r="3">
       <x v="2"/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="6"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="10" baseItem="0" numFmtId="164"/>
@@ -6997,11 +7598,47 @@
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="1">
+  <chartFormats count="4">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -7363,7 +8000,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>145</v>
       </c>
     </row>
@@ -7645,7 +8282,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>171</v>
       </c>
     </row>
@@ -13900,110 +14537,124 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7698054C-9202-4D00-8BAF-E2CD8CC28B1A}">
-  <dimension ref="A3:B14"/>
+  <dimension ref="A3:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="16.77734375" customWidth="1"/>
+    <col min="1" max="5" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B5" s="27">
+        <v>64894.25</v>
+      </c>
+      <c r="C5" s="27">
+        <v>70</v>
+      </c>
+      <c r="D5" s="27">
+        <v>1</v>
+      </c>
+      <c r="E5" s="27">
         <v>64965.25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B6" s="27">
+        <v>64894.25</v>
+      </c>
+      <c r="C6" s="27">
+        <v>70</v>
+      </c>
+      <c r="D6" s="27">
+        <v>1</v>
+      </c>
+      <c r="E6" s="27">
         <v>64965.25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
         <v>169</v>
-      </c>
-      <c r="B6" s="27">
-        <v>30301.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
-        <v>13</v>
       </c>
       <c r="B7" s="27">
         <v>30270.25</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
-        <v>31</v>
+      <c r="C7" s="27">
+        <v>35</v>
+      </c>
+      <c r="D7" s="27">
+        <v>-4</v>
+      </c>
+      <c r="E7" s="27">
+        <v>30301.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>170</v>
       </c>
       <c r="B8" s="27">
+        <v>34624</v>
+      </c>
+      <c r="C8" s="27">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
-        <v>39</v>
+      <c r="D8" s="27">
+        <v>5</v>
+      </c>
+      <c r="E8" s="27">
+        <v>34664</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>166</v>
       </c>
       <c r="B9" s="27">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="B10" s="27">
-        <v>34664</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="27">
-        <v>34624</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="27">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="B14" s="27">
+        <v>64894.25</v>
+      </c>
+      <c r="C9" s="27">
+        <v>70</v>
+      </c>
+      <c r="D9" s="27">
+        <v>1</v>
+      </c>
+      <c r="E9" s="27">
         <v>64965.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refixed issue based on what was shared in class
</commit_message>
<xml_diff>
--- a/section2/ChrisF_ExcelHomework.xlsx
+++ b/section2/ChrisF_ExcelHomework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Code\SavvyCoders\Homework\section2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06B761C-D333-47AD-B823-53DE7946482F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E25693-A0FA-4282-9857-EA1E6CEA209E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31350" yWindow="2550" windowWidth="21600" windowHeight="13185" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="173">
   <si>
     <t>Expenses</t>
   </si>
@@ -558,9 +558,6 @@
   </si>
   <si>
     <t>Citi Card</t>
-  </si>
-  <si>
-    <t>Column Labels</t>
   </si>
 </sst>
 </file>
@@ -680,7 +677,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -740,6 +737,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2031,12 +2034,109 @@
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="88000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="threePt" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:contourClr>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4472C4">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:alpha val="50000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -2077,22 +2177,7 @@
           </a:sp3d>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2177,22 +2262,7 @@
           </a:sp3d>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2277,22 +2347,7 @@
           </a:sp3d>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2404,11 +2459,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Payments!$B$3:$B$4</c:f>
+              <c:f>Payments!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B1</c:v>
+                  <c:v>Total</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2510,14 +2565,34 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Payments!$A$5:$A$9</c:f>
+              <c:f>Payments!$A$4:$A$14</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>B1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>B2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>B1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>B2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Jan</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="3">
                     <c:v>Feb</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2536,15 +2611,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Payments!$B$5:$B$9</c:f>
+              <c:f>Payments!$B$4:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>30270.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>34624</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2552,318 +2639,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-182A-4B9E-BE8B-70E6072E849D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Payments!$C$3:$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>B2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:alpha val="88000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-            <a:scene3d>
-              <a:camera prst="orthographicFront"/>
-              <a:lightRig rig="threePt" dir="t"/>
-            </a:scene3d>
-            <a:sp3d prstMaterial="flat">
-              <a:contourClr>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:contourClr>
-            </a:sp3d>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ED7D31">
-                  <a:alpha val="30000"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:sysClr val="window" lastClr="FFFFFF">
-                    <a:alpha val="50000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Payments!$A$5:$A$9</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="2"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Jan</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Feb</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Qtr1</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2012</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Payments!$C$5:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>35</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AFD9-4B07-A4FD-940BEFA09790}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Payments!$D$3:$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:alpha val="88000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-            <a:scene3d>
-              <a:camera prst="orthographicFront"/>
-              <a:lightRig rig="threePt" dir="t"/>
-            </a:scene3d>
-            <a:sp3d prstMaterial="flat">
-              <a:contourClr>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:contourClr>
-            </a:sp3d>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="A5A5A5">
-                  <a:alpha val="30000"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:sysClr val="window" lastClr="FFFFFF">
-                    <a:alpha val="50000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Payments!$A$5:$A$9</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="2"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Jan</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Feb</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Qtr1</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2012</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Payments!$D$5:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AFD9-4B07-A4FD-940BEFA09790}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4960,15 +4735,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>172403</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:colOff>101918</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>142876</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>53341</xdr:rowOff>
+      <xdr:colOff>74296</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7491,7 +7266,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5BD7C614-9F3D-4318-8A3D-E92C5709C969}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField showAll="0"/>
@@ -7499,7 +7274,7 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" numFmtId="43" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="4">
         <item x="0"/>
         <item x="1"/>
@@ -7548,12 +7323,13 @@
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="3">
+  <rowFields count="4">
     <field x="10"/>
     <field x="9"/>
     <field x="8"/>
+    <field x="6"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="11">
     <i>
       <x v="2"/>
     </i>
@@ -7563,29 +7339,33 @@
     <i r="2">
       <x v="1"/>
     </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="3">
+      <x v="2"/>
+    </i>
     <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="3">
+      <x/>
+    </i>
+    <i r="3">
+      <x v="1"/>
+    </i>
+    <i r="3">
       <x v="2"/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
-  <colFields count="1">
-    <field x="6"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="10" baseItem="0" numFmtId="164"/>
@@ -14537,10 +14317,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7698054C-9202-4D00-8BAF-E2CD8CC28B1A}">
-  <dimension ref="A3:E9"/>
+  <dimension ref="A3:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14548,113 +14328,99 @@
     <col min="1" max="5" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
         <v>168</v>
       </c>
+      <c r="B4" s="27">
+        <v>64965.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>167</v>
+      </c>
       <c r="B5" s="27">
-        <v>64894.25</v>
-      </c>
-      <c r="C5" s="27">
-        <v>70</v>
-      </c>
-      <c r="D5" s="27">
-        <v>1</v>
-      </c>
-      <c r="E5" s="27">
         <v>64965.25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
-        <v>167</v>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>169</v>
       </c>
       <c r="B6" s="27">
-        <v>64894.25</v>
-      </c>
-      <c r="C6" s="27">
-        <v>70</v>
-      </c>
-      <c r="D6" s="27">
-        <v>1</v>
-      </c>
-      <c r="E6" s="27">
-        <v>64965.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
-        <v>169</v>
+        <v>30301.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>13</v>
       </c>
       <c r="B7" s="27">
         <v>30270.25</v>
       </c>
-      <c r="C7" s="27">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="27">
         <v>35</v>
       </c>
-      <c r="D7" s="27">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="27">
         <v>-4</v>
       </c>
-      <c r="E7" s="27">
-        <v>30301.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B10" s="27">
+        <v>34664</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="27">
         <v>34624</v>
       </c>
-      <c r="C8" s="27">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="27">
         <v>35</v>
       </c>
-      <c r="D8" s="27">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="27">
         <v>5</v>
       </c>
-      <c r="E8" s="27">
-        <v>34664</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="B9" s="27">
-        <v>64894.25</v>
-      </c>
-      <c r="C9" s="27">
-        <v>70</v>
-      </c>
-      <c r="D9" s="27">
-        <v>1</v>
-      </c>
-      <c r="E9" s="27">
+      <c r="B14" s="27">
         <v>64965.25</v>
       </c>
     </row>

</xml_diff>